<commit_message>
freeze first column in "Staff Percentages" report.
</commit_message>
<xml_diff>
--- a/GRis/Content/ExcelTemplates/StaffPercentagesMonthlyReportTemplate.xlsx
+++ b/GRis/Content/ExcelTemplates/StaffPercentagesMonthlyReportTemplate.xlsx
@@ -373,7 +373,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>